<commit_message>
Modified FrontEnd and Enabled 6 models
</commit_message>
<xml_diff>
--- a/SpotifyPersonalityPredictor/ProjectSolution/SpotifyPersonalityDataset.xlsx
+++ b/SpotifyPersonalityPredictor/ProjectSolution/SpotifyPersonalityDataset.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikon\SpotifyPersonalityPredictor\ProjectSolution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikon\SpotifyPersonalityProject\SpotifyPersonalityPredictor\ProjectSolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC226C0-7369-497C-93BD-9B73894ED8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DA451D-C3C0-435B-BF16-EE9B77B59804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="348" windowWidth="11532" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7236" yWindow="420" windowWidth="11532" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -88,10 +88,8 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -194,7 +192,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -226,27 +224,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -278,24 +258,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -472,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,52 +500,52 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.55507274198652812</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="C2">
-        <v>0.59180356925719924</v>
+        <v>0.59</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>-9.5506335729463316</v>
+        <v>-9.6</v>
       </c>
       <c r="F2">
-        <v>8.9733523215335328E-2</v>
+        <v>0.09</v>
       </c>
       <c r="G2">
-        <v>0.32665878205804949</v>
+        <v>0.32900000000000001</v>
       </c>
       <c r="H2">
-        <v>0.18318093198643709</v>
+        <v>0.18</v>
       </c>
       <c r="I2">
-        <v>0.18221057823590589</v>
+        <v>0.182</v>
       </c>
       <c r="J2">
-        <v>0.42290996157149918</v>
+        <v>0.42</v>
       </c>
       <c r="K2">
-        <v>120.71362424160201</v>
+        <v>121</v>
       </c>
       <c r="L2">
         <v>4</v>
       </c>
       <c r="M2">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="N2">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="O2">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="P2">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="Q2">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -591,55 +553,214 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.55518996847933166</v>
+        <v>0.61</v>
       </c>
       <c r="C3">
-        <v>0.59029326136866467</v>
+        <v>0.67</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>-9.5912488507148659</v>
+        <v>-6.6</v>
       </c>
       <c r="F3">
-        <v>9.2238605142655861E-2</v>
+        <v>0.1</v>
       </c>
       <c r="G3">
-        <v>0.32650296695631348</v>
+        <v>0.21</v>
       </c>
       <c r="H3">
-        <v>0.18478930768454049</v>
+        <v>0.04</v>
       </c>
       <c r="I3">
-        <v>0.1821014812004951</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="J3">
-        <v>0.42341458892170419</v>
+        <v>0.5</v>
       </c>
       <c r="K3">
-        <v>120.8838833012705</v>
+        <v>125</v>
       </c>
       <c r="L3">
         <v>4</v>
       </c>
       <c r="M3">
+        <v>8</v>
+      </c>
+      <c r="N3">
+        <v>6</v>
+      </c>
+      <c r="O3">
+        <v>6</v>
+      </c>
+      <c r="P3">
+        <v>9</v>
+      </c>
+      <c r="Q3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C4">
+        <v>0.75</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>-5.9</v>
+      </c>
+      <c r="F4">
+        <v>0.09</v>
+      </c>
+      <c r="G4">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="H4">
+        <v>0.06</v>
+      </c>
+      <c r="I4">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="J4">
+        <v>0.49</v>
+      </c>
+      <c r="K4">
+        <v>127</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <v>8</v>
+      </c>
+      <c r="O4">
+        <v>4</v>
+      </c>
+      <c r="P4">
+        <v>8</v>
+      </c>
+      <c r="Q4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C5">
+        <v>0.54</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>-10.7</v>
+      </c>
+      <c r="F5">
+        <v>0.09</v>
+      </c>
+      <c r="G5">
+        <v>0.376</v>
+      </c>
+      <c r="H5">
+        <v>0.23</v>
+      </c>
+      <c r="I5">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="J5">
+        <v>0.39</v>
+      </c>
+      <c r="K5">
+        <v>119</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
         <v>5</v>
       </c>
-      <c r="N3">
-        <v>8</v>
-      </c>
-      <c r="O3">
-        <v>8</v>
-      </c>
-      <c r="P3">
+      <c r="N5">
+        <v>8</v>
+      </c>
+      <c r="O5">
+        <v>8</v>
+      </c>
+      <c r="P5">
         <v>5</v>
       </c>
-      <c r="Q3">
+      <c r="Q5">
         <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.83</v>
+      </c>
+      <c r="C6">
+        <v>0.65</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>-5.2</v>
+      </c>
+      <c r="F6">
+        <v>0.06</v>
+      </c>
+      <c r="G6">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="J6">
+        <v>0.34</v>
+      </c>
+      <c r="K6">
+        <v>136</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>6</v>
+      </c>
+      <c r="N6">
+        <v>7</v>
+      </c>
+      <c r="O6">
+        <v>7</v>
+      </c>
+      <c r="P6">
+        <v>6</v>
+      </c>
+      <c r="Q6">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>